<commit_message>
script complete. TODO: validation
</commit_message>
<xml_diff>
--- a/InputData/messages.xlsx
+++ b/InputData/messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattd\IdeaProjects\BoG\hdg-chatbot\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424B3A8C-FE1D-4D3F-868D-EBE426A528DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED014FE-A190-4831-AA67-538D842F60FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E4F2BC1-98AF-4436-ABD2-BA309168EB1C}"/>
+    <workbookView xWindow="10068" yWindow="1284" windowWidth="10836" windowHeight="8964" xr2:uid="{6E4F2BC1-98AF-4436-ABD2-BA309168EB1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -63,16 +63,88 @@
     <t>image</t>
   </si>
   <si>
-    <t>no image</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
     <t>image 2</t>
   </si>
   <si>
-    <t>no image 2</t>
+    <t>KEYWORDS</t>
+  </si>
+  <si>
+    <t>ISQUESTION</t>
+  </si>
+  <si>
+    <t>(Welcome Message) What would you like to learn about? 1. (emoji) Exercise - brief description2. (emoji) WASH- brief description3. (emoji) Nutrition-brief description4. (emoji) Maternal Infant Care-brief description5. (emoji) Mental Health- brief description</t>
+  </si>
+  <si>
+    <t>2, 3, 4, 5, 6</t>
+  </si>
+  <si>
+    <t>Exercise</t>
+  </si>
+  <si>
+    <t>WASH</t>
+  </si>
+  <si>
+    <t>Nutrition</t>
+  </si>
+  <si>
+    <t>Maternal Infant Care</t>
+  </si>
+  <si>
+    <t>Mental Health</t>
+  </si>
+  <si>
+    <t>next exercise</t>
+  </si>
+  <si>
+    <t>next wash</t>
+  </si>
+  <si>
+    <t>next nutrition</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>low data wash</t>
+  </si>
+  <si>
+    <t>low data nutrition</t>
+  </si>
+  <si>
+    <t>low data welcome</t>
+  </si>
+  <si>
+    <t>low data exercise</t>
+  </si>
+  <si>
+    <t>low data maternal health</t>
+  </si>
+  <si>
+    <t>low data mental halth</t>
+  </si>
+  <si>
+    <t>low data exer 2</t>
+  </si>
+  <si>
+    <t>low data wash 2</t>
+  </si>
+  <si>
+    <t>low daya nutrition 2</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>google.com</t>
   </si>
 </sst>
 </file>
@@ -424,15 +496,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA6A2BB-9C23-4233-A3B0-E435AB329052}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,48 +534,248 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>2</v>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>29</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing isQuestion to messageType
</commit_message>
<xml_diff>
--- a/InputData/messages.xlsx
+++ b/InputData/messages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattd\IdeaProjects\BoG\hdg-chatbot\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexb8z/Downloads/hdg-chatbot/InputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9261FDD6-C97F-45C5-AB4F-F4A5DFF785F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BD9873-AC10-2349-BE0E-0E70587DCFAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5532" yWindow="2304" windowWidth="15948" windowHeight="8964" xr2:uid="{6E4F2BC1-98AF-4436-ABD2-BA309168EB1C}"/>
+    <workbookView xWindow="5540" yWindow="2300" windowWidth="15940" windowHeight="8960" xr2:uid="{6E4F2BC1-98AF-4436-ABD2-BA309168EB1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -69,9 +60,6 @@
     <t>KEYWORDS</t>
   </si>
   <si>
-    <t>ISQUESTION</t>
-  </si>
-  <si>
     <t>(Welcome Message) What would you like to learn about? 1. (emoji) Exercise - brief description2. (emoji) WASH- brief description3. (emoji) Nutrition-brief description4. (emoji) Maternal Infant Care-brief description5. (emoji) Mental Health- brief description</t>
   </si>
   <si>
@@ -145,6 +133,21 @@
   </si>
   <si>
     <t>google.com</t>
+  </si>
+  <si>
+    <t>MESSAGETYPE</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>final-message</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>splitting</t>
   </si>
 </sst>
 </file>
@@ -499,20 +502,20 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,21 +541,21 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -561,18 +564,21 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -587,21 +593,21 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -613,21 +619,21 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>9</v>
@@ -639,21 +645,21 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -665,18 +671,18 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -691,18 +697,18 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -717,21 +723,21 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -743,21 +749,21 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="I9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -769,10 +775,10 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" t="b">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>